<commit_message>
The Cake is a Lie Update
</commit_message>
<xml_diff>
--- a/The Cake is a Lie.xlsx
+++ b/The Cake is a Lie.xlsx
@@ -1,21 +1,15 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="19126"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <fileVersion appName="xl" lastEdited="5" lowestEdited="6" rupBuild="9302"/>
   <workbookPr/>
-  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-    <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Processor\"/>
-    </mc:Choice>
-  </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="12_ncr:500000_{CE3751DF-4443-4C7C-9DE0-4A7D27545DCA}" xr6:coauthVersionLast="31" xr6:coauthVersionMax="31" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="20490" windowHeight="7545" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="20490" windowHeight="7545"/>
   </bookViews>
   <sheets>
     <sheet name="Hoja1" sheetId="1" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="152511"/>
+  <calcPr calcId="144525"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -25,7 +19,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="69" uniqueCount="48">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="210" uniqueCount="118">
   <si>
     <t>op</t>
   </si>
@@ -169,12 +163,222 @@
   </si>
   <si>
     <t>RESTORE</t>
+  </si>
+  <si>
+    <t>BA</t>
+  </si>
+  <si>
+    <t>1000</t>
+  </si>
+  <si>
+    <t>Branch</t>
+  </si>
+  <si>
+    <t>Always</t>
+  </si>
+  <si>
+    <t>1</t>
+  </si>
+  <si>
+    <t>BN</t>
+  </si>
+  <si>
+    <t>0000</t>
+  </si>
+  <si>
+    <t>Never</t>
+  </si>
+  <si>
+    <t>0</t>
+  </si>
+  <si>
+    <t>BNE</t>
+  </si>
+  <si>
+    <t>1001</t>
+  </si>
+  <si>
+    <t>on</t>
+  </si>
+  <si>
+    <t>Not</t>
+  </si>
+  <si>
+    <t>Equal</t>
+  </si>
+  <si>
+    <t>not</t>
+  </si>
+  <si>
+    <t>Z</t>
+  </si>
+  <si>
+    <t>BE</t>
+  </si>
+  <si>
+    <t>0001</t>
+  </si>
+  <si>
+    <t>BG</t>
+  </si>
+  <si>
+    <t>1010</t>
+  </si>
+  <si>
+    <t>Greater</t>
+  </si>
+  <si>
+    <t>(Z</t>
+  </si>
+  <si>
+    <t>or</t>
+  </si>
+  <si>
+    <t>(N</t>
+  </si>
+  <si>
+    <t>xor</t>
+  </si>
+  <si>
+    <t>V))</t>
+  </si>
+  <si>
+    <t>BLE</t>
+  </si>
+  <si>
+    <t>0010</t>
+  </si>
+  <si>
+    <t>Less</t>
+  </si>
+  <si>
+    <t>V)</t>
+  </si>
+  <si>
+    <t>BGE</t>
+  </si>
+  <si>
+    <t>1011</t>
+  </si>
+  <si>
+    <t>BL</t>
+  </si>
+  <si>
+    <t>0011</t>
+  </si>
+  <si>
+    <t>N</t>
+  </si>
+  <si>
+    <t>V</t>
+  </si>
+  <si>
+    <t>BGU</t>
+  </si>
+  <si>
+    <t>1100</t>
+  </si>
+  <si>
+    <t>Unsigned</t>
+  </si>
+  <si>
+    <t>(C</t>
+  </si>
+  <si>
+    <t>Z)</t>
+  </si>
+  <si>
+    <t>BLEU</t>
+  </si>
+  <si>
+    <t>0100</t>
+  </si>
+  <si>
+    <t>BCC</t>
+  </si>
+  <si>
+    <t>1101</t>
+  </si>
+  <si>
+    <t>Carry</t>
+  </si>
+  <si>
+    <t>Clear</t>
+  </si>
+  <si>
+    <t>(Greater</t>
+  </si>
+  <si>
+    <t>than</t>
+  </si>
+  <si>
+    <t>Equal,</t>
+  </si>
+  <si>
+    <t>Unsigned)</t>
+  </si>
+  <si>
+    <t>C</t>
+  </si>
+  <si>
+    <t>BCS</t>
+  </si>
+  <si>
+    <t>0101</t>
+  </si>
+  <si>
+    <t>Set</t>
+  </si>
+  <si>
+    <t>(Less</t>
+  </si>
+  <si>
+    <t>than,</t>
+  </si>
+  <si>
+    <t>BPOS</t>
+  </si>
+  <si>
+    <t>1110</t>
+  </si>
+  <si>
+    <t>Positive</t>
+  </si>
+  <si>
+    <t>BNEG</t>
+  </si>
+  <si>
+    <t>0110</t>
+  </si>
+  <si>
+    <t>Negative</t>
+  </si>
+  <si>
+    <t>BVC</t>
+  </si>
+  <si>
+    <t>1111</t>
+  </si>
+  <si>
+    <t>Overflow</t>
+  </si>
+  <si>
+    <t>BVS</t>
+  </si>
+  <si>
+    <t>0111</t>
+  </si>
+  <si>
+    <t>opcode</t>
+  </si>
+  <si>
+    <t>cond</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <fonts count="1" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
@@ -219,7 +423,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="6">
+  <cellXfs count="8">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
@@ -234,6 +438,8 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -294,7 +500,7 @@
     </a:clrScheme>
     <a:fontScheme name="Office">
       <a:majorFont>
-        <a:latin typeface="Calibri Light" panose="020F0302020204030204"/>
+        <a:latin typeface="Calibri Light"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -329,7 +535,7 @@
         <a:font script="Geor" typeface="Sylfaen"/>
       </a:majorFont>
       <a:minorFont>
-        <a:latin typeface="Calibri" panose="020F0502020204030204"/>
+        <a:latin typeface="Calibri"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -506,23 +712,23 @@
   <a:extraClrSchemeLst/>
   <a:extLst>
     <a:ext uri="{05A4C25C-085E-4340-85A3-A5531E510DB2}">
-      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
+      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" xmlns="" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
     </a:ext>
   </a:extLst>
 </a:theme>
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="C2:F25"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="C2:S25"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A6" workbookViewId="0">
-      <selection activeCell="F23" sqref="F23:F24"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="D6" sqref="D6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <sheetData>
-    <row r="2" spans="3:5" x14ac:dyDescent="0.25">
+    <row r="2" spans="3:19" x14ac:dyDescent="0.25">
       <c r="C2" s="1" t="s">
         <v>0</v>
       </c>
@@ -532,8 +738,31 @@
       <c r="E2" s="1" t="s">
         <v>2</v>
       </c>
-    </row>
-    <row r="3" spans="3:5" x14ac:dyDescent="0.25">
+      <c r="G2" s="7" t="s">
+        <v>53</v>
+      </c>
+      <c r="H2" s="7" t="s">
+        <v>54</v>
+      </c>
+      <c r="I2" s="7" t="s">
+        <v>50</v>
+      </c>
+      <c r="J2" s="7" t="s">
+        <v>55</v>
+      </c>
+      <c r="K2" s="7" t="s">
+        <v>56</v>
+      </c>
+      <c r="L2" s="6"/>
+      <c r="M2" s="6"/>
+      <c r="N2" s="6"/>
+      <c r="O2" s="6"/>
+      <c r="P2" s="6"/>
+      <c r="Q2" s="6"/>
+      <c r="R2" s="6"/>
+      <c r="S2" s="6"/>
+    </row>
+    <row r="3" spans="3:19" x14ac:dyDescent="0.25">
       <c r="C3" s="2" t="s">
         <v>45</v>
       </c>
@@ -543,8 +772,33 @@
       <c r="E3" s="2" t="s">
         <v>6</v>
       </c>
-    </row>
-    <row r="4" spans="3:5" x14ac:dyDescent="0.25">
+      <c r="G3" s="7" t="s">
+        <v>64</v>
+      </c>
+      <c r="H3" s="7" t="s">
+        <v>65</v>
+      </c>
+      <c r="I3" s="7" t="s">
+        <v>50</v>
+      </c>
+      <c r="J3" s="7" t="s">
+        <v>59</v>
+      </c>
+      <c r="K3" s="7" t="s">
+        <v>61</v>
+      </c>
+      <c r="L3" s="7" t="s">
+        <v>63</v>
+      </c>
+      <c r="M3" s="6"/>
+      <c r="N3" s="6"/>
+      <c r="O3" s="6"/>
+      <c r="P3" s="6"/>
+      <c r="Q3" s="6"/>
+      <c r="R3" s="6"/>
+      <c r="S3" s="6"/>
+    </row>
+    <row r="4" spans="3:19" x14ac:dyDescent="0.25">
       <c r="C4" s="2" t="s">
         <v>45</v>
       </c>
@@ -554,8 +808,45 @@
       <c r="E4" s="2" t="s">
         <v>19</v>
       </c>
-    </row>
-    <row r="5" spans="3:5" x14ac:dyDescent="0.25">
+      <c r="G4" s="7" t="s">
+        <v>74</v>
+      </c>
+      <c r="H4" s="7" t="s">
+        <v>75</v>
+      </c>
+      <c r="I4" s="7" t="s">
+        <v>50</v>
+      </c>
+      <c r="J4" s="7" t="s">
+        <v>59</v>
+      </c>
+      <c r="K4" s="7" t="s">
+        <v>76</v>
+      </c>
+      <c r="L4" s="7" t="s">
+        <v>70</v>
+      </c>
+      <c r="M4" s="7" t="s">
+        <v>61</v>
+      </c>
+      <c r="N4" s="7" t="s">
+        <v>63</v>
+      </c>
+      <c r="O4" s="7" t="s">
+        <v>70</v>
+      </c>
+      <c r="P4" s="7" t="s">
+        <v>71</v>
+      </c>
+      <c r="Q4" s="7" t="s">
+        <v>72</v>
+      </c>
+      <c r="R4" s="6" t="s">
+        <v>77</v>
+      </c>
+      <c r="S4" s="6"/>
+    </row>
+    <row r="5" spans="3:19" x14ac:dyDescent="0.25">
       <c r="C5" s="2" t="s">
         <v>45</v>
       </c>
@@ -565,8 +856,37 @@
       <c r="E5" s="2" t="s">
         <v>16</v>
       </c>
-    </row>
-    <row r="6" spans="3:5" x14ac:dyDescent="0.25">
+      <c r="G5" s="7" t="s">
+        <v>80</v>
+      </c>
+      <c r="H5" s="7" t="s">
+        <v>81</v>
+      </c>
+      <c r="I5" s="7" t="s">
+        <v>50</v>
+      </c>
+      <c r="J5" s="7" t="s">
+        <v>59</v>
+      </c>
+      <c r="K5" s="7" t="s">
+        <v>76</v>
+      </c>
+      <c r="L5" s="7" t="s">
+        <v>82</v>
+      </c>
+      <c r="M5" s="7" t="s">
+        <v>72</v>
+      </c>
+      <c r="N5" s="7" t="s">
+        <v>83</v>
+      </c>
+      <c r="O5" s="6"/>
+      <c r="P5" s="6"/>
+      <c r="Q5" s="6"/>
+      <c r="R5" s="6"/>
+      <c r="S5" s="6"/>
+    </row>
+    <row r="6" spans="3:19" x14ac:dyDescent="0.25">
       <c r="C6" s="2" t="s">
         <v>45</v>
       </c>
@@ -576,8 +896,43 @@
       <c r="E6" s="2" t="s">
         <v>21</v>
       </c>
-    </row>
-    <row r="7" spans="3:5" x14ac:dyDescent="0.25">
+      <c r="G6" s="7" t="s">
+        <v>89</v>
+      </c>
+      <c r="H6" s="7" t="s">
+        <v>90</v>
+      </c>
+      <c r="I6" s="7" t="s">
+        <v>50</v>
+      </c>
+      <c r="J6" s="7" t="s">
+        <v>59</v>
+      </c>
+      <c r="K6" s="7" t="s">
+        <v>76</v>
+      </c>
+      <c r="L6" s="7" t="s">
+        <v>70</v>
+      </c>
+      <c r="M6" s="7" t="s">
+        <v>61</v>
+      </c>
+      <c r="N6" s="7" t="s">
+        <v>86</v>
+      </c>
+      <c r="O6" s="7" t="s">
+        <v>87</v>
+      </c>
+      <c r="P6" s="7" t="s">
+        <v>70</v>
+      </c>
+      <c r="Q6" s="7" t="s">
+        <v>88</v>
+      </c>
+      <c r="R6" s="6"/>
+      <c r="S6" s="6"/>
+    </row>
+    <row r="7" spans="3:19" x14ac:dyDescent="0.25">
       <c r="C7" s="2" t="s">
         <v>45</v>
       </c>
@@ -587,8 +942,41 @@
       <c r="E7" s="2" t="s">
         <v>10</v>
       </c>
-    </row>
-    <row r="8" spans="3:5" x14ac:dyDescent="0.25">
+      <c r="G7" s="7" t="s">
+        <v>100</v>
+      </c>
+      <c r="H7" s="7" t="s">
+        <v>101</v>
+      </c>
+      <c r="I7" s="7" t="s">
+        <v>50</v>
+      </c>
+      <c r="J7" s="7" t="s">
+        <v>59</v>
+      </c>
+      <c r="K7" s="7" t="s">
+        <v>93</v>
+      </c>
+      <c r="L7" s="7" t="s">
+        <v>102</v>
+      </c>
+      <c r="M7" s="7" t="s">
+        <v>103</v>
+      </c>
+      <c r="N7" s="7" t="s">
+        <v>104</v>
+      </c>
+      <c r="O7" s="7" t="s">
+        <v>98</v>
+      </c>
+      <c r="P7" s="7" t="s">
+        <v>99</v>
+      </c>
+      <c r="Q7" s="6"/>
+      <c r="R7" s="6"/>
+      <c r="S7" s="6"/>
+    </row>
+    <row r="8" spans="3:19" x14ac:dyDescent="0.25">
       <c r="C8" s="2" t="s">
         <v>45</v>
       </c>
@@ -598,8 +986,33 @@
       <c r="E8" s="2" t="s">
         <v>26</v>
       </c>
-    </row>
-    <row r="9" spans="3:5" x14ac:dyDescent="0.25">
+      <c r="G8" s="7" t="s">
+        <v>108</v>
+      </c>
+      <c r="H8" s="7" t="s">
+        <v>109</v>
+      </c>
+      <c r="I8" s="7" t="s">
+        <v>50</v>
+      </c>
+      <c r="J8" s="7" t="s">
+        <v>59</v>
+      </c>
+      <c r="K8" s="7" t="s">
+        <v>110</v>
+      </c>
+      <c r="L8" s="7" t="s">
+        <v>82</v>
+      </c>
+      <c r="M8" s="6"/>
+      <c r="N8" s="6"/>
+      <c r="O8" s="6"/>
+      <c r="P8" s="6"/>
+      <c r="Q8" s="6"/>
+      <c r="R8" s="6"/>
+      <c r="S8" s="6"/>
+    </row>
+    <row r="9" spans="3:19" x14ac:dyDescent="0.25">
       <c r="C9" s="2" t="s">
         <v>45</v>
       </c>
@@ -609,8 +1022,35 @@
       <c r="E9" s="2" t="s">
         <v>18</v>
       </c>
-    </row>
-    <row r="10" spans="3:5" x14ac:dyDescent="0.25">
+      <c r="G9" s="7" t="s">
+        <v>114</v>
+      </c>
+      <c r="H9" s="7" t="s">
+        <v>115</v>
+      </c>
+      <c r="I9" s="7" t="s">
+        <v>50</v>
+      </c>
+      <c r="J9" s="7" t="s">
+        <v>59</v>
+      </c>
+      <c r="K9" s="7" t="s">
+        <v>113</v>
+      </c>
+      <c r="L9" s="7" t="s">
+        <v>102</v>
+      </c>
+      <c r="M9" s="7" t="s">
+        <v>83</v>
+      </c>
+      <c r="N9" s="6"/>
+      <c r="O9" s="6"/>
+      <c r="P9" s="6"/>
+      <c r="Q9" s="6"/>
+      <c r="R9" s="6"/>
+      <c r="S9" s="6"/>
+    </row>
+    <row r="10" spans="3:19" x14ac:dyDescent="0.25">
       <c r="C10" s="2" t="s">
         <v>45</v>
       </c>
@@ -620,8 +1060,31 @@
       <c r="E10" s="2" t="s">
         <v>24</v>
       </c>
-    </row>
-    <row r="11" spans="3:5" x14ac:dyDescent="0.25">
+      <c r="G10" s="7" t="s">
+        <v>48</v>
+      </c>
+      <c r="H10" s="7" t="s">
+        <v>49</v>
+      </c>
+      <c r="I10" s="7" t="s">
+        <v>50</v>
+      </c>
+      <c r="J10" s="7" t="s">
+        <v>51</v>
+      </c>
+      <c r="K10" s="7" t="s">
+        <v>52</v>
+      </c>
+      <c r="L10" s="6"/>
+      <c r="M10" s="6"/>
+      <c r="N10" s="6"/>
+      <c r="O10" s="6"/>
+      <c r="P10" s="6"/>
+      <c r="Q10" s="6"/>
+      <c r="R10" s="6"/>
+      <c r="S10" s="6"/>
+    </row>
+    <row r="11" spans="3:19" x14ac:dyDescent="0.25">
       <c r="C11" s="2" t="s">
         <v>45</v>
       </c>
@@ -631,8 +1094,37 @@
       <c r="E11" s="2" t="s">
         <v>12</v>
       </c>
-    </row>
-    <row r="12" spans="3:5" x14ac:dyDescent="0.25">
+      <c r="G11" s="7" t="s">
+        <v>57</v>
+      </c>
+      <c r="H11" s="7" t="s">
+        <v>58</v>
+      </c>
+      <c r="I11" s="7" t="s">
+        <v>50</v>
+      </c>
+      <c r="J11" s="7" t="s">
+        <v>59</v>
+      </c>
+      <c r="K11" s="7" t="s">
+        <v>60</v>
+      </c>
+      <c r="L11" s="7" t="s">
+        <v>61</v>
+      </c>
+      <c r="M11" s="7" t="s">
+        <v>62</v>
+      </c>
+      <c r="N11" s="7" t="s">
+        <v>63</v>
+      </c>
+      <c r="O11" s="6"/>
+      <c r="P11" s="6"/>
+      <c r="Q11" s="6"/>
+      <c r="R11" s="6"/>
+      <c r="S11" s="6"/>
+    </row>
+    <row r="12" spans="3:19" x14ac:dyDescent="0.25">
       <c r="C12" s="2" t="s">
         <v>45</v>
       </c>
@@ -642,8 +1134,43 @@
       <c r="E12" s="2" t="s">
         <v>30</v>
       </c>
-    </row>
-    <row r="13" spans="3:5" x14ac:dyDescent="0.25">
+      <c r="G12" s="7" t="s">
+        <v>66</v>
+      </c>
+      <c r="H12" s="7" t="s">
+        <v>67</v>
+      </c>
+      <c r="I12" s="7" t="s">
+        <v>50</v>
+      </c>
+      <c r="J12" s="7" t="s">
+        <v>59</v>
+      </c>
+      <c r="K12" s="7" t="s">
+        <v>68</v>
+      </c>
+      <c r="L12" s="7" t="s">
+        <v>62</v>
+      </c>
+      <c r="M12" s="7" t="s">
+        <v>69</v>
+      </c>
+      <c r="N12" s="7" t="s">
+        <v>70</v>
+      </c>
+      <c r="O12" s="7" t="s">
+        <v>71</v>
+      </c>
+      <c r="P12" s="7" t="s">
+        <v>72</v>
+      </c>
+      <c r="Q12" s="7" t="s">
+        <v>73</v>
+      </c>
+      <c r="R12" s="6"/>
+      <c r="S12" s="6"/>
+    </row>
+    <row r="13" spans="3:19" x14ac:dyDescent="0.25">
       <c r="C13" s="2" t="s">
         <v>45</v>
       </c>
@@ -653,8 +1180,43 @@
       <c r="E13" s="2" t="s">
         <v>14</v>
       </c>
-    </row>
-    <row r="14" spans="3:5" x14ac:dyDescent="0.25">
+      <c r="G13" s="7" t="s">
+        <v>78</v>
+      </c>
+      <c r="H13" s="7" t="s">
+        <v>79</v>
+      </c>
+      <c r="I13" s="7" t="s">
+        <v>50</v>
+      </c>
+      <c r="J13" s="7" t="s">
+        <v>59</v>
+      </c>
+      <c r="K13" s="7" t="s">
+        <v>68</v>
+      </c>
+      <c r="L13" s="7" t="s">
+        <v>70</v>
+      </c>
+      <c r="M13" s="7" t="s">
+        <v>61</v>
+      </c>
+      <c r="N13" s="7" t="s">
+        <v>62</v>
+      </c>
+      <c r="O13" s="7" t="s">
+        <v>71</v>
+      </c>
+      <c r="P13" s="7" t="s">
+        <v>72</v>
+      </c>
+      <c r="Q13" s="7" t="s">
+        <v>77</v>
+      </c>
+      <c r="R13" s="6"/>
+      <c r="S13" s="6"/>
+    </row>
+    <row r="14" spans="3:19" x14ac:dyDescent="0.25">
       <c r="C14" s="2" t="s">
         <v>45</v>
       </c>
@@ -664,8 +1226,41 @@
       <c r="E14" s="2" t="s">
         <v>28</v>
       </c>
-    </row>
-    <row r="15" spans="3:5" x14ac:dyDescent="0.25">
+      <c r="G14" s="7" t="s">
+        <v>84</v>
+      </c>
+      <c r="H14" s="7" t="s">
+        <v>85</v>
+      </c>
+      <c r="I14" s="7" t="s">
+        <v>50</v>
+      </c>
+      <c r="J14" s="7" t="s">
+        <v>59</v>
+      </c>
+      <c r="K14" s="7" t="s">
+        <v>68</v>
+      </c>
+      <c r="L14" s="7" t="s">
+        <v>86</v>
+      </c>
+      <c r="M14" s="7" t="s">
+        <v>62</v>
+      </c>
+      <c r="N14" s="7" t="s">
+        <v>87</v>
+      </c>
+      <c r="O14" s="7" t="s">
+        <v>70</v>
+      </c>
+      <c r="P14" s="7" t="s">
+        <v>88</v>
+      </c>
+      <c r="Q14" s="6"/>
+      <c r="R14" s="6"/>
+      <c r="S14" s="6"/>
+    </row>
+    <row r="15" spans="3:19" x14ac:dyDescent="0.25">
       <c r="C15" s="2" t="s">
         <v>45</v>
       </c>
@@ -675,8 +1270,47 @@
       <c r="E15" s="1" t="s">
         <v>4</v>
       </c>
-    </row>
-    <row r="16" spans="3:5" x14ac:dyDescent="0.25">
+      <c r="G15" s="7" t="s">
+        <v>91</v>
+      </c>
+      <c r="H15" s="7" t="s">
+        <v>92</v>
+      </c>
+      <c r="I15" s="7" t="s">
+        <v>50</v>
+      </c>
+      <c r="J15" s="7" t="s">
+        <v>59</v>
+      </c>
+      <c r="K15" s="7" t="s">
+        <v>93</v>
+      </c>
+      <c r="L15" s="7" t="s">
+        <v>94</v>
+      </c>
+      <c r="M15" s="7" t="s">
+        <v>95</v>
+      </c>
+      <c r="N15" s="7" t="s">
+        <v>96</v>
+      </c>
+      <c r="O15" s="7" t="s">
+        <v>70</v>
+      </c>
+      <c r="P15" s="7" t="s">
+        <v>97</v>
+      </c>
+      <c r="Q15" s="7" t="s">
+        <v>98</v>
+      </c>
+      <c r="R15" s="6" t="s">
+        <v>62</v>
+      </c>
+      <c r="S15" s="6" t="s">
+        <v>99</v>
+      </c>
+    </row>
+    <row r="16" spans="3:19" x14ac:dyDescent="0.25">
       <c r="C16" s="2" t="s">
         <v>45</v>
       </c>
@@ -686,8 +1320,35 @@
       <c r="E16" s="1" t="s">
         <v>36</v>
       </c>
-    </row>
-    <row r="17" spans="3:6" x14ac:dyDescent="0.25">
+      <c r="G16" s="7" t="s">
+        <v>105</v>
+      </c>
+      <c r="H16" s="7" t="s">
+        <v>106</v>
+      </c>
+      <c r="I16" s="7" t="s">
+        <v>50</v>
+      </c>
+      <c r="J16" s="7" t="s">
+        <v>59</v>
+      </c>
+      <c r="K16" s="7" t="s">
+        <v>107</v>
+      </c>
+      <c r="L16" s="7" t="s">
+        <v>62</v>
+      </c>
+      <c r="M16" s="7" t="s">
+        <v>82</v>
+      </c>
+      <c r="N16" s="6"/>
+      <c r="O16" s="6"/>
+      <c r="P16" s="6"/>
+      <c r="Q16" s="6"/>
+      <c r="R16" s="6"/>
+      <c r="S16" s="6"/>
+    </row>
+    <row r="17" spans="3:19" x14ac:dyDescent="0.25">
       <c r="C17" s="2" t="s">
         <v>45</v>
       </c>
@@ -697,8 +1358,37 @@
       <c r="E17" s="1" t="s">
         <v>34</v>
       </c>
-    </row>
-    <row r="18" spans="3:6" x14ac:dyDescent="0.25">
+      <c r="G17" s="7" t="s">
+        <v>111</v>
+      </c>
+      <c r="H17" s="7" t="s">
+        <v>112</v>
+      </c>
+      <c r="I17" s="7" t="s">
+        <v>50</v>
+      </c>
+      <c r="J17" s="7" t="s">
+        <v>59</v>
+      </c>
+      <c r="K17" s="7" t="s">
+        <v>113</v>
+      </c>
+      <c r="L17" s="7" t="s">
+        <v>94</v>
+      </c>
+      <c r="M17" s="7" t="s">
+        <v>62</v>
+      </c>
+      <c r="N17" s="7" t="s">
+        <v>83</v>
+      </c>
+      <c r="O17" s="6"/>
+      <c r="P17" s="6"/>
+      <c r="Q17" s="6"/>
+      <c r="R17" s="6"/>
+      <c r="S17" s="6"/>
+    </row>
+    <row r="18" spans="3:19" x14ac:dyDescent="0.25">
       <c r="C18" s="2" t="s">
         <v>45</v>
       </c>
@@ -708,8 +1398,27 @@
       <c r="E18" s="1" t="s">
         <v>32</v>
       </c>
-    </row>
-    <row r="19" spans="3:6" x14ac:dyDescent="0.25">
+      <c r="G18" s="3" t="s">
+        <v>116</v>
+      </c>
+      <c r="H18" s="3" t="s">
+        <v>117</v>
+      </c>
+      <c r="I18" s="3" t="s">
+        <v>2</v>
+      </c>
+      <c r="J18" s="6"/>
+      <c r="K18" s="6"/>
+      <c r="L18" s="6"/>
+      <c r="M18" s="6"/>
+      <c r="N18" s="6"/>
+      <c r="O18" s="6"/>
+      <c r="P18" s="6"/>
+      <c r="Q18" s="6"/>
+      <c r="R18" s="6"/>
+      <c r="S18" s="6"/>
+    </row>
+    <row r="19" spans="3:19" x14ac:dyDescent="0.25">
       <c r="C19" s="2" t="s">
         <v>45</v>
       </c>
@@ -720,7 +1429,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="20" spans="3:6" x14ac:dyDescent="0.25">
+    <row r="20" spans="3:19" x14ac:dyDescent="0.25">
       <c r="C20" s="2" t="s">
         <v>45</v>
       </c>
@@ -731,7 +1440,7 @@
         <v>42</v>
       </c>
     </row>
-    <row r="21" spans="3:6" x14ac:dyDescent="0.25">
+    <row r="21" spans="3:19" x14ac:dyDescent="0.25">
       <c r="C21" s="2" t="s">
         <v>45</v>
       </c>
@@ -742,7 +1451,7 @@
         <v>40</v>
       </c>
     </row>
-    <row r="22" spans="3:6" x14ac:dyDescent="0.25">
+    <row r="22" spans="3:19" x14ac:dyDescent="0.25">
       <c r="C22" s="2" t="s">
         <v>45</v>
       </c>
@@ -753,7 +1462,7 @@
         <v>38</v>
       </c>
     </row>
-    <row r="23" spans="3:6" x14ac:dyDescent="0.25">
+    <row r="23" spans="3:19" x14ac:dyDescent="0.25">
       <c r="C23" s="2" t="s">
         <v>45</v>
       </c>
@@ -767,7 +1476,7 @@
         <v>44</v>
       </c>
     </row>
-    <row r="24" spans="3:6" x14ac:dyDescent="0.25">
+    <row r="24" spans="3:19" x14ac:dyDescent="0.25">
       <c r="C24" s="2" t="s">
         <v>45</v>
       </c>
@@ -781,10 +1490,13 @@
         <v>46</v>
       </c>
     </row>
-    <row r="25" spans="3:6" x14ac:dyDescent="0.25">
+    <row r="25" spans="3:19" x14ac:dyDescent="0.25">
       <c r="C25" s="4"/>
     </row>
   </sheetData>
+  <sortState ref="G2:S18">
+    <sortCondition ref="H2"/>
+  </sortState>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>
   <ignoredErrors>

</xml_diff>